<commit_message>
Add Width attribute in Fields>Field|Gap|Packet|Group, values Default|BestFit|Number (multiply by 100).
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample01-from-code.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample01-from-code.xlsx
@@ -6,6 +6,7 @@
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
+    <sheet name="ssss" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory'!$A$1:$E$1</definedName>
@@ -299,6 +300,13 @@
     <sheetView workbookViewId="0" showGridLines="1" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.88098199026925" customWidth="1"/>
+    <col min="2" max="2" width="10.7065026419503" customWidth="1"/>
+    <col min="3" max="3" width="11.5720160348075" customWidth="1"/>
+    <col min="4" max="4" width="8.09870910644531" customWidth="1"/>
+    <col min="5" max="5" width="8.77802440098354" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
@@ -389,4 +397,15 @@
     <oddHeader>&amp;CInventory</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add changes in xsd model, cs model classes, for support column width fields, and add support for Trim and TrimMode in groups fields, Add sample 13 in iEngineSamples (works with columns width)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample01-from-code.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/xlsx/EPPlus/sample01-from-code.xlsx
@@ -6,7 +6,6 @@
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
-    <sheet name="ssss" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory'!$A$1:$E$1</definedName>
@@ -300,13 +299,6 @@
     <sheetView workbookViewId="0" showGridLines="1" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="6.88098199026925" customWidth="1"/>
-    <col min="2" max="2" width="10.7065026419503" customWidth="1"/>
-    <col min="3" max="3" width="11.5720160348075" customWidth="1"/>
-    <col min="4" max="4" width="8.09870910644531" customWidth="1"/>
-    <col min="5" max="5" width="8.77802440098354" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
@@ -397,15 +389,4 @@
     <oddHeader>&amp;CInventory</oddHeader>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>